<commit_message>
Added autotype for marbles on stream scoring system
</commit_message>
<xml_diff>
--- a/marbleracing/season2/backup.xlsx
+++ b/marbleracing/season2/backup.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="20">
   <si>
     <t>Flair</t>
   </si>
@@ -63,13 +63,19 @@
     <t>1st (+30)</t>
   </si>
   <si>
+    <t>2nd (+25)</t>
+  </si>
+  <si>
+    <t>2nd (+99)</t>
+  </si>
+  <si>
     <t>MoscaMye</t>
   </si>
   <si>
     <t>2nd</t>
   </si>
   <si>
-    <t>2nd (+25)</t>
+    <t>1st (+100)</t>
   </si>
 </sst>
 </file>
@@ -93,18 +99,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -119,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -127,7 +127,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,7 +481,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="1">
-        <v>120</v>
+        <v>184</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>14</v>
@@ -491,10 +490,10 @@
         <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -502,23 +501,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1">
-        <v>75</v>
-      </c>
-      <c r="E3" s="3"/>
+        <v>180</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="F3" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -582,23 +583,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1">
-        <v>75</v>
-      </c>
-      <c r="E2" s="3"/>
+        <v>180</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="F2" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -612,7 +615,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="1">
-        <v>120</v>
+        <v>184</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>14</v>
@@ -621,10 +624,10 @@
         <v>14</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -688,23 +691,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1">
-        <v>75</v>
-      </c>
-      <c r="E2" s="3"/>
+        <v>180</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="F2" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -718,7 +723,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="1">
-        <v>120</v>
+        <v>184</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>14</v>
@@ -727,10 +732,10 @@
         <v>14</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prepared website for marble racing
</commit_message>
<xml_diff>
--- a/marbleracing/season2/backup.xlsx
+++ b/marbleracing/season2/backup.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
   <si>
     <t>Flair</t>
   </si>
@@ -52,30 +52,6 @@
   </si>
   <si>
     <t>Race 8</t>
-  </si>
-  <si>
-    <t>Zokalyx</t>
-  </si>
-  <si>
-    <t>1st</t>
-  </si>
-  <si>
-    <t>1st (+30)</t>
-  </si>
-  <si>
-    <t>2nd (+25)</t>
-  </si>
-  <si>
-    <t>2nd (+99)</t>
-  </si>
-  <si>
-    <t>MoscaMye</t>
-  </si>
-  <si>
-    <t>2nd</t>
-  </si>
-  <si>
-    <t>1st (+100)</t>
   </si>
 </sst>
 </file>
@@ -421,13 +397,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="8" width="10.7109375" style="1" customWidth="1"/>
+    <col min="1" max="4" width="10.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="4" width="15.7109375" customWidth="1"/>
   </cols>
@@ -470,58 +446,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="1">
-        <v>27</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="1">
-        <v>184</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1">
-        <v>180</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -529,13 +453,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="8" width="10.7109375" style="1" customWidth="1"/>
+    <col min="1" max="4" width="10.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="4" width="15.7109375" customWidth="1"/>
   </cols>
@@ -578,58 +502,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="1">
-        <v>180</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="1">
-        <v>27</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1">
-        <v>184</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -637,13 +509,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="8" width="10.7109375" style="1" customWidth="1"/>
+    <col min="1" max="4" width="10.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="4" width="15.7109375" customWidth="1"/>
   </cols>
@@ -686,58 +558,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="1">
-        <v>180</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="1">
-        <v>27</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1">
-        <v>184</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
race 1 and various fixes/improvements
</commit_message>
<xml_diff>
--- a/marbleracing/season2/backup.xlsx
+++ b/marbleracing/season2/backup.xlsx
@@ -75,15 +75,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -91,16 +97,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -403,46 +421,45 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="10.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="4" width="15.7109375" customWidth="1"/>
+    <col min="3" max="12" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -459,46 +476,45 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="10.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="4" width="15.7109375" customWidth="1"/>
+    <col min="3" max="12" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -515,46 +531,45 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="10.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="4" width="15.7109375" customWidth="1"/>
+    <col min="3" max="12" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>